<commit_message>
Fixed some issues with Excel template.xlsx. Added an information about calculation.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\UPS_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BB7841-1E5B-4487-82E6-63457CF609B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA631CA-4274-4A55-9918-F28AA1417238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43B12854-8764-4A86-89BD-BD8C93AD66B3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Модель: </t>
   </si>
@@ -64,13 +64,271 @@
   </si>
   <si>
     <t>Расчётное время работы с выбранной конфигурацией:</t>
+  </si>
+  <si>
+    <t>Алгоритм расчёта:</t>
+  </si>
+  <si>
+    <t>Время автономной работы рассчитывается исходя из следующей формулы:</t>
+  </si>
+  <si>
+    <t>где:</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ИБП</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – ёмкость аккумуляторных батарей, встроенных в источник бесперебойного питания, Вт·ч. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>С</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>АКБ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>– ёмкость аккумуляторных батарей, встроенных в аккумуляторное расширение для источника бесперебойного питания, Вт·ч.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>АКР</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – количество аккумуляторных расширений, подключаемых к источнику бесперебойного питания.</t>
+    </r>
+  </si>
+  <si>
+    <t>60 – число минут в часе.</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – потребляемая мощность нагрузки, Вт.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – коэффициент неполноты разряда АКБ. Зависит от времени автономной работы и может быть приближённо вычислен исходя из аппроксимации степенной функцией общего графика зависимости ёмкости аккумуляторных батарей от времени разряда: </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Уравнение коэффициента неполноты разряда АКБ с формулой аппроксимации степенной функцией имеет вид: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">где </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> – расчётное время автономной работы, без учёта коэффициента неполноты разряда АКБ, час.</t>
+  </si>
+  <si>
+    <t>Ёмкость аккумуляторных батарей, встроенных в источник бесперебойного питания и аккумуляторное расширение измеряется в Ватт-часах (Вт·ч) и вычисляется по формулам:</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>АКБ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – число аккумуляторных батарей в ИБП или расширении;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>АКБ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – ёмкость одной аккумуляторной батареи, А·ч;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>АКБ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – напряжение на выходе аккумуляторной батареи, В. </t>
+    </r>
+  </si>
+  <si>
+    <t>где:
+T – расчётное время работы от аккумуляторов, мин.</t>
+  </si>
+  <si>
+    <r>
+      <t>КПД</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ИБП</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – КПД инвертора источника бесперебойного питания. Как правило, составляет 0,8 (80%) для линейно-интерактивных ИБП и 0,9 (90%) для ИБП с двойным преобразованием рода тока (онлайн).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +345,38 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -164,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -174,6 +464,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -190,6 +501,427 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3924300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{734544F6-5A83-921C-96CC-C01623D40D0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1238250" y="5076825"/>
+          <a:ext cx="2686050" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3562350</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 1" descr="Ð·Ð°Ð²Ð¸ÑÐ¸Ð¼Ð¾ÑÑÑ ÐµÐ¼ÐºÐ¾ÑÑÐ¸ Ð°ÐºÐºÑÐ¼ÑÐ»ÑÑÐ¾ÑÐ° Ð¾Ñ Ð²ÑÐµÐ¼ÐµÐ½Ð¸ ÑÐ°Ð·ÑÑÐ´Ð°">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4883FE56-5C40-0D79-58D8-BBA6A41696D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="704850" y="9105899"/>
+          <a:ext cx="2857500" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3143250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66FF63CD-1094-1736-CDF8-DF4493BE729E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="11925300"/>
+          <a:ext cx="2219325" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6697D7B5-1C0A-C54D-A92F-38C3C9D07F24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="30099000"/>
+          <a:ext cx="85725" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Рисунок 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95456A5-CDD7-3AA8-C6FB-30F49B4E1B00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="31099125"/>
+          <a:ext cx="1590675" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E55699-5388-E76F-7789-CFEF89F51543}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="31299150"/>
+          <a:ext cx="1571625" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,10 +1224,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,26 +1301,151 @@
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:2" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="43" spans="1:2" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed incorrect captions in Excel and text field
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\UPS_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA631CA-4274-4A55-9918-F28AA1417238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77EBD45-B0D5-4B68-96E2-AB3837197A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43B12854-8764-4A86-89BD-BD8C93AD66B3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43B12854-8764-4A86-89BD-BD8C93AD66B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Расчёт" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t xml:space="preserve">Модель: </t>
   </si>
   <si>
-    <t>Потребляемая мощность:</t>
-  </si>
-  <si>
     <t>Ёмкость одной АКБ в ИБП:</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
       </rPr>
       <t xml:space="preserve"> – КПД инвертора источника бесперебойного питания. Как правило, составляет 0,8 (80%) для линейно-интерактивных ИБП и 0,9 (90%) для ИБП с двойным преобразованием рода тока (онлайн).</t>
     </r>
+  </si>
+  <si>
+    <t>Мощность нагрузки:</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1255,7 +1255,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -1263,7 +1263,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -1303,7 +1303,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1320,12 +1320,12 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="12"/>
     </row>
@@ -1334,56 +1334,56 @@
     </row>
     <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="7"/>
     </row>
     <row r="29" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="11"/>
     </row>
     <row r="30" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="11"/>
     </row>
     <row r="32" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="11"/>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="12"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="11"/>
     </row>
     <row r="35" spans="1:2" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="11"/>
     </row>
     <row r="43" spans="1:2" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1391,22 +1391,22 @@
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1414,22 +1414,22 @@
     </row>
     <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>